<commit_message>
cleaned emails with nltk
</commit_message>
<xml_diff>
--- a/Katrina.xlsx
+++ b/Katrina.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sundial\Uni President Emails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmas\OneDrive\Desktop\Sundial\Uni President Emails\Columbia-President-Emails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE84FF1C-E40F-4FED-A33C-E5B24D8D269F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743525A9-8C9D-4818-8BDB-5AE2626655A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
   <si>
     <t>Title</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Affirming our Mission</t>
   </si>
   <si>
-    <t>A Message for Our Community About Election Week</t>
-  </si>
-  <si>
     <t>Supporting Our Community</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>11/25/2024 15:44</t>
   </si>
   <si>
-    <t>11/1/2024 13:10</t>
-  </si>
-  <si>
     <t>10/1/2024 8:30</t>
   </si>
   <si>
@@ -196,29 +190,23 @@
     <t>8/14/2024 20:19</t>
   </si>
   <si>
-    <t>Dear fellow members of the Columbia community:
-As I have shared with you, we have been working this year on critical 
+    <t>A Message from Katrina Armstrong</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>As I have shared with you, we have been working this year on critical 
 priorities for our University, which you can find on our “Fulfilling Our 
-Commitments” website 
-&lt;https://president.columbia.edu/content/fulfilling-our-commitments  &gt;. We 
-have shared our progress on several of our key priorities with the U.S. 
-Department of Education, U.S. Department of Health and Human Services, 
-and the General Services Administration. You can find that document here 
-&lt;https://president.columbia.edu/sites/default/files/content/03.21.2025   
-Columbia - FINAL.pdf&gt;, and on our website 
-&lt;https://president.columbia.edu/content/fulfilling-our-commitments  &gt;.
-This past year has been one of enormous progress, where our community of 
-thoughtful faculty, students, and stakeholders has shaped a principled 
-and methodical approach to meeting the moment's challenges. Our response 
-to the government agencies outlines the substantive work we've been 
-doing over the last academic year to advance our mission, ensure 
+Commitments” website. We have shared our progress on several of our key priorities with the U.S. Department of Education, U.S. Department of Health and Human Services, and the General Services Administration. You can find that document here and on our website.
+This past year has been one of enormous progress, where our community of thoughtful faculty, students, and stakeholders has shaped a principled 
+and methodical approach to meeting the moment's challenges. Our response to the government agencies outlines the substantive work we've been doing over the last academic year to advance our mission, ensure 
 uninterrupted academic activities, and make every student, faculty, and 
 staff member safe and welcome on our campus.
 We have much to be proud of as a community, and it has been a privilege 
 to share our progress and plans. In the spirit of great American 
 universities, we expect Columbians to engage in robust debate and 
-discussion about our way forward, and we welcome it as an opportunity to 
-shape the future of Columbia.
+discussion about our way forward, and we welcome it as an opportunity to shape the future of Columbia.
 The way Columbia and Columbians have been portrayed is hard to reckon 
 with. We have challenges, yes, but they do not define us. We are a 
 community of scholars who have deep respect for each other and our 
@@ -228,23 +216,15 @@
 and brilliant.
 At all times, we are guided by our values, putting academic freedom, 
 free expression, open inquiry, and respect for all at the fore of every 
-decision we make.
-Standing together for Columbia,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-Many of you have seen the March 13th letter we received from U.S. 
+decision we make.</t>
+  </si>
+  <si>
+    <t>Many of you have seen the March 13th letter we received from U.S. 
 Department of Education, U.S. Department of Health and Human Services, 
 and the General Services Administration outlining preconditions for 
 “continued financial relationships with the United States government.”
 Understandably, many inside and outside of our community have voiced 
-concern, asking how we will respond. Some have examined each 
-pre-condition on its own, weighing the acceptable versus the 
-intolerable. Many bristle at the very idea that an institution like 
-ours—an institution whose very value is premised on free inquiry and 
-free expression—should ever be subject to such a list.
+concern, asking how we will respond. Some have examined each pre-condition on its own, weighing the acceptable versus the intolerable. Many bristle at the very idea that an institution like ours—an institution whose very value is premised on free inquiry and free expression—should ever be subject to such a list.
 Let me be clear about our path forward: it is our utmost responsibility 
 to uphold and deliver on our academic mission, always. We are committed 
 to doing what's right for Columbia and will not waver from our 
@@ -255,14 +235,10 @@
 this campus community needs to address. Antisemitism, harassment, and 
 discrimination of any kind are unacceptable and imperil both our sense 
 of community as well as our very academic mission.
-We are extremely proud of the progress we have made on many important 
-issues on campus, following the priorities I outlined at the start of 
-each semester. Addressing issues of antisemitism, harassment, and 
+We are extremely proud of the progress we have made on many important issues on campus, following the priorities I outlined at the start of each semester. Addressing issues of antisemitism, harassment, and 
 discrimination has been a critical focus for me, with steps ranging from 
 the creation of a new Office of Institutional Equity to the work of our 
-Campus Collaborative on building community and enhancing dialogue across 
-our campuses. We have clarified and improved implementation of our 
-University Rules and discipline processes. Most recently, we have 
+Campus Collaborative on building community and enhancing dialogue across our campuses. We have clarified and improved implementation of our University Rules and discipline processes. Most recently, we have 
 focused on making substantive improvements to our Public Safety 
 capabilities, so that we can safely expand campus access. Throughout 
 this, my commitment is to ensure that our students and student groups 
@@ -273,10 +249,7 @@
 behavior imperils their commitment to free expression and academic 
 freedom in the classroom. Fixing these harms is part of Columbia's 
 healing process and just last week, we announced a new policy on 
-anti-doxing and online harassment. In addition, all of our 
-student-facing offices are working around the clock to support the needs 
-of our students. We are committed to implementing policies and 
-procedures that prioritize safety in and outside of the classroom.
+anti-doxing and online harassment. In addition, all of our student-facing offices are working around the clock to support the needs of our students. We are committed to implementing policies and procedures that prioritize safety in and outside of the classroom.
 Amidst a historically charged and divisive political atmosphere, 
 academic institutions, of all places, must be able to operate with 
 wisdom and deliberation, even as our various constituencies are moved to 
@@ -299,27 +272,17 @@
 While we can feel the progress on our campus, there is certainly more 
 work to be done, and we are eager to share our progress with you. We'll 
 soon be launching a webpage that will contain regular updates on all the 
-progress we're making across all these areas.
-Thank you for standing for Columbia,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear fellow members of our Columbia community:
-Over the last months, components of the federal government have 
+progress we're making across all these areas.</t>
+  </si>
+  <si>
+    <t>Over the last months, components of the federal government have 
 announced investigations into our University, creating great concern 
 across our community and the nation. The stakes are high not only for 
 Columbia, but for every college and university in this country. Columbia 
 finds itself yet again leading the nation and we will do what is right.
 Our University is defined by the principles of academic freedom, open 
 inquiry, and respect for all. These principles are fundamental to 
-Columbia's broader mandate of advancing the betterment of our community, 
-our city, our country, and the world. We will defend these principles 
-with courage and determination. It is because of these values that 
-Columbia serves the world so well. From Alexander Hamilton to Dwight D. 
-Eisenhower to the present, we teach, we heal, we innovate, and we create 
-knowledge. To damage Columbia is to weaken American ingenuity and 
-leadership.
+Columbia's broader mandate of advancing the betterment of our community, our city, our country, and the world. We will defend these principles with courage and determination. It is because of these values that Columbia serves the world so well. From Alexander Hamilton to Dwight D. Eisenhower to the present, we teach, we heal, we innovate, and we create knowledge. To damage Columbia is to weaken American ingenuity and leadership.
 This is a critical moment for higher education in this country. The 
 freedom of universities is tied to the freedom of every other 
 institution in a thriving democracy. In this moment, I want to 
@@ -335,27 +298,32 @@
 not to further divide us. Since I stepped into this role, we have worked 
 tirelessly to address both internal and external concerns, to build a 
 better Columbia. As we continue this hard work of repairing and 
-strengthening our community, we must preserve our ability to decide what 
-is right for Columbians and the people we serve. We will decide how to 
-do that together as a community.
+strengthening our community, we must preserve our ability to decide what is right for Columbians and the people we serve. We will decide how to do that together as a community.
 I am incredibly fortunate to have spent my career at great universities. 
 I take the responsibility of serving as your leader at this time as an 
 honor and privilege. For 270 years we have transcended our challenges 
-and I know we will continue to do so.
-Standing together for Columbia,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York
+and I know we will continue to do so.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am writing heartbroken to inform you that we had federal agents from the Department of Homeland Security (DHS) in two University residences tonight. No one was arrested or detained. No items were removed, and no further action was taken.
+Federal agents from the DHS served Columbia University with two judicial
+search warrants signed by a federal magistrate judge authorizing DHS to
+enter non-public areas of the University and conduct searches of two
+student rooms.
+The University has a clear protocol in place. Consistent with this protocol, our longstanding practice, and the practices of cities and institutions throughout the country, the University requires that law enforcement have a judicial warrant to enter non-public University areas, including residential University buildings. Tonight, that threshold was met, and the University is obligated to comply with the law. Our University Public Safety was present at all times.
+Columbia continues to make every effort to ensure that our campus,
+students, faculty, and staff are safe. Columbia is committed to upholding
+the law, and we expect city, state, and federal agencies to do the same.
+I understand the immense stress our community is under. Despite the
+unprecedented challenges, Columbia University will remain a place where the pursuit of knowledge is cherished and fiercely protected, where the rule of law and due process is respected and never taken for granted, and where all members of our community are valued and able to thrive. These are the principles we uphold and that guide us every day.
+For students in need of support, I've included a list of University
+resources below.
 </t>
   </si>
   <si>
-    <t>Dear fellow members of the Columbia community:
-Like most colleges and universities in the United States, Columbia 
+    <t>Like most colleges and universities in the United States, Columbia 
 University is home to faculty, staff, and students from all over the 
-world. Some of our community members are on temporary visas; others are 
-green-card holders or naturalized citizens. These Columbians contribute 
-to our University and to our nation in countless ways; through their 
-energy, creativity, innovation, and dedication to academic excellence in 
-the service of advancing our society and world.
+world. Some of our community members are on temporary visas; others are green-card holders or naturalized citizens. These Columbians contribute to our University and to our nation in countless ways; through their energy, creativity, innovation, and dedication to academic excellence in the service of advancing our society and world.
 Columbia University welcomes all those who honor us with their talent, 
 experience, and ambition. We support them whether they came to the 
 United States as children, as students, as refugees from war or 
@@ -388,16 +356,10 @@
 and other institutions of higher learning come together to affirm and 
 openly reassert these long-standing principles, in support of our 
 international faculty, staff, and students, and for our collective 
-well-being.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York
-Angela Olinto
-Provost, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-I want to reiterate the principles that have guided me over my thirty 
+well-being.</t>
+  </si>
+  <si>
+    <t>I want to reiterate the principles that have guided me over my thirty 
 years as a faculty member and are guiding me today.
 First, I stand by my students, all of my students. I support their right 
 to express their views and to participate in open and respectful 
@@ -416,14 +378,10 @@
 discord and collaboration out of conflict. I have no doubt that the days 
 and weeks ahead are going to be extremely difficult. The best I can 
 promise is that I will never stray from these principles and that I will 
-work tirelessly to defend our remarkable, singular institution.
-Best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-Columbia's mission is to teach, create, and advance knowledge. For over 
+work tirelessly to defend our remarkable, singular institution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columbia's mission is to teach, create, and advance knowledge. For over 
 270 years, that mission has been grounded in an enduring and essential 
 commitment to freedom of expression, open inquiry, and generous, 
 respectful debate.
@@ -441,13 +399,9 @@
 are committed to working with the federal government to address their 
 legitimate concerns. To that end, Columbia can, and will, continue to 
 take serious action toward combatting antisemitism on our campus 
-&lt;https://president.columbia.edu/content/combatting-antisemitism&gt;.
 This is our number one priority.
-Today's announcement will undoubtedly create anxiety and concern for our 
-entire community. These impacts will touch nearly every corner of the 
-University. But it is during periods like this that our collective 
-dedication to this institution and our mission takes on critical 
-importance.
+Today's announcement will undoubtedly create anxiety and concern for our entire community. These impacts will touch nearly every corner of the 
+University. But it is during periods like this that our collective dedication to this institution and our mission takes on critical importance.
 Our north star has not changed. We are committed to education and 
 research that will benefit our nation and our world. We believe in the 
 power of knowledge to drive progress and improve lives. Our mission as a 
@@ -506,27 +460,18 @@
 We must hold firm and summon the courage to meet this moment with 
 determination, integrity and humility. I look forward to working with 
 all of you to achieve exactly this.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-The challenges we face in this moment are no secret. Along with other 
+</t>
+  </si>
+  <si>
+    <t>The challenges we face in this moment are no secret. Along with other 
 leaders of our University, I have been traveling to Capitol Hill to 
-advocate for Columbia and for higher education with members of Congress 
-who are shaping the future of our nation. We are still figuring out how 
-to navigate the ongoing changes in the federal government's approach to 
-its funding of research and other policies affecting higher education. I 
-want to share some thoughts on the situation and a few conclusions I've 
-drawn from my congressional visits.
+advocate for Columbia and for higher education with members of Congress who are shaping the future of our nation. We are still figuring out how to navigate the ongoing changes in the federal government's approach to its funding of research and other policies affecting higher education. I want to share some thoughts on the situation and a few conclusions I've drawn from my congressional visits.
 First, I believe this period of uncertainty will continue for some time. 
 We must work together as we face these new challenges and the new 
 realities that emerge from them. Many of you have reached out to provide 
 new ideas and insight, to express concern or anger, or to offer your 
 help and collaboration. Your outreach and responses speak to the depth 
-of the Columbia community's commitment to its mission. Please know that 
-for several months our leadership has been actively preparing for this 
+of the Columbia community's commitment to its mission. Please know that for several months our leadership has been actively preparing for this 
 changing federal policy environment, working with experts and peer 
 institutions, evaluating potential impacts, and undertaking strategic 
 planning. We cannot predict all that will unfold, but we are actively 
@@ -551,15 +496,25 @@
 updates with our community on developments and the actions we are 
 undertaking, but we welcome your ideas as well. I have no doubt that our 
 Columbia community is up to rising to meet this moment. If we work 
-together we can emerge from this time stronger than ever.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-In response to the recent memo from the Office of Management and Budget 
-pausing federal funding, I want to take a moment to reiterate our 
+together we can emerge from this time stronger than ever.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In September, I announced the creation of a President's Advisory 
+Committee on Institutional Voice to provide me with a set of recommendations on the proper role of institutional voice in advancing Columbia's academic mission and its commitment to open inquiry and free expression. I am writing now with an update on this critical work.
+I am pleased to share that the Committee has begun its work, including 
+developing an engagement strategy and holding meetings with faculty, 
+students, administrators, and staff from across the University. The 
+Committee anticipates completing its work and providing a report to me 
+by the end of the current academic year. The full roster of Committee 
+members is listed below. They include thoughtful and experienced faculty 
+from departments and schools across our campuses, and I am very grateful to them for agreeing to do this challenging and urgently needed work.
+The Committee has also established a website, which will be a resource for further information and updates. It will welcome input and feedback from members of the Columbia community, so please get in touch with them at institutionalvoice@columbia.edu if you would like to share your thoughts and insights.
+I offer my deepest thanks to the two distinguished Co-Chairs, Daniel 
+Abebe, Dean of Columbia Law School and Lucy G. Moses Professor of Law, and Mark Mazower, Ira D. Wallach Professor of World Order Studies, and to all the members of the Committee. We are very fortunate to have their deliberations guide us in this important project.
+</t>
+  </si>
+  <si>
+    <t>In response to the recent memo from the Office of Management and Budget pausing federal funding, I want to take a moment to reiterate our 
 unwavering commitment to the core mission and principles that define us.
 Over the past several months, our leadership team has been actively 
 planning for a variety of scenarios, including this one. In 
@@ -570,37 +525,69 @@
 At the heart of our work are our students, our patients, our faculty, 
 and our research. Each of these groups are fundamental not only to the 
 future of our University but also to the advancement of knowledge and 
-society as a whole. Our commitment to their success remains resolute. We 
-understand that this moment may prompt concern, but it is in times such 
-as these that our strength shines brightest.
-Columbia has weathered difficult moments throughout our history, drawing 
-on the resolve and resilience of this community to emerge stronger each 
-time. Today, we stand at another such moment. It is a time for us to 
-come together, to respond thoughtfully, and to demonstrate our ability 
-to adapt with integrity and with our mission at the fore.
+society as a whole. Our commitment to their success remains resolute. We understand that this moment may prompt concern, but it is in times such as these that our strength shines brightest.
+Columbia has weathered difficult moments throughout our history, drawing on the resolve and resilience of this community to emerge stronger each time. Today, we stand at another such moment. It is a time for us to come together, to respond thoughtfully, and to demonstrate our ability to adapt with integrity and with our mission at the fore.
 This will be a dynamic period, and we will keep you informed as new 
 developments unfold. We will be as transparent as we can in our 
 communications and in our decision-making processes, as we continue to 
 uphold the values that make our University a beacon of excellence.
-Thank you for your continued dedication to our shared mission.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-For those who have returned to Morningside this week, you have seen that 
-our CUID requirement for access to the Morningside campus is still in 
+Thank you for your continued dedication to our shared mission.</t>
+  </si>
+  <si>
+    <t>Dear Columbia Community,
+I write to you at a challenging moment for our community. Columbia 
+University exists to serve the United States and the world, by teaching, 
+creating, and advancing knowledge. We pursue that mission through 
+freedom of expression, open inquiry, a wide range of perspectives, and 
+respectful debate. These are Columbia's values, they are America's 
+values, they are essential to a functioning democracy, and we will fight 
+for them. We do this for our students and for our future.
+Here is what that means in this particular moment:
+  *We will work tirelessly to fulfill our mission. We are taking a
+    methodical and thoughtful approach to addressing the multitude of
+    challenges ahead of us. We are engaged with several federal agencies
+    and are doing all we can to be responsive to their legitimate
+    concerns and to take corrective action, under the law, to restore
+    funding.
+  *We will support our community. I understand the distress that many
+    of you are feeling about the presence of U.S. Immigration and
+    Customs Enforcement (ICE) agents in the streets around campus. I
+    feel it too and am working with our team to manage the response.
+    Resources for students are listed below.
+  *We will follow the law, as has always been the case, and rumors
+    suggesting that any member of Columbia leadership requested the
+    presence of U.S. Immigration and Customs Enforcement (ICE) agents on
+    or near campus are false. It remains the long-standing practice of
+    the University, and the practice of cities and institutions
+    throughout the country, that law enforcement must have a judicial
+    warrant to enter non-public University areas, including residential
+    University buildings.
+  *We are deeply committed to freedom of speech as a fundamental
+    value that we must uphold as a community—citizens and non-citizens
+    alike. Vigorous and open debate, consistent with our rules, is
+    central to achieving our academic mission. We must welcome the
+    widest possible range of ideas, perspectives, and life experiences
+    from all members of our community whether American or International.
+    Our mission at Columbia also requires that we treat one another with
+    respect, which enables us to disagree without being disagreeable. We
+    need to do so in an environment free from discrimination.
+I am proud of Columbia's unwavering commitment to excellence, and our 
+historic and ongoing contributions to the United States and the world, 
+from technology, to medicine, to the humanities, to the laws 
+underpinning our democracy itself. I ask for your continued support and 
+patience. The only way to navigate this moment is together, as a united 
+community.
+All eyes are on Columbia at present. It falls to us to ensure our 
+University, and indeed the values of higher education more broadly, 
+survive and thrive.</t>
+  </si>
+  <si>
+    <t>For those who have returned to Morningside this week, you have seen that our CUID requirement for access to the Morningside campus is still in 
 place. All of us appreciate that an open campus supports our academic 
 pursuits, enriches the experience of our students, and connects us to 
 our neighbors, New York City, and the world beyond. Perhaps most 
-importantly, an open campus symbolizes our commitment to an open mind 
-and open dialogue, fundamental tenets of our mission and our history. We 
-have made progress toward the goal of fully reopening the Morningside 
-campus and moving beyond access requirements, but we still have more 
-work to do.
-Over the last months, we have gained a much deeper understanding of how 
-many students, faculty, and staff did not feel welcome or safe on the 
+importantly, an open campus symbolizes our commitment to an open mind and open dialogue, fundamental tenets of our mission and our history. We have made progress toward the goal of fully reopening the Morningside campus and moving beyond access requirements, but we still have more work to do.
+Over the last months, we have gained a much deeper understanding of how many students, faculty, and staff did not feel welcome or safe on the 
 Morningside campus last spring, whether from the disruption of the 
 encampments and associated protests and incidents or the actions and 
 presence of the NYPD. Unfortunately, recent events have shown that our 
@@ -635,41 +622,25 @@
     reported. Masking makes it difficult for Public Safety to
     distinguish between outside demonstrators and members of our
     university community.
-  * We have convened a Morningside Campus Access Advisory Committee to
-    review information, including input from external partners, evaluate
+  * We have convened a Morningside Campus Access Advisory Committee to review information, including input from external partners, evaluate
     the tradeoffs, and weigh in on strategies to ensure that all groups
     feel welcome and safe on campus when the gates are open.
-We will provide additional updates on this *work here* 
-&lt;https://publicsafety.columbia.edu/content/morningside-campus-access-updates&gt;. 
-Please continue to share your feedback and provide suggestions at the 
-Inclusive Public Safety Advisory Committee website 
-&lt;https://universitylife.columbia.edu/inclusive-public-safety&gt;. Our goal 
+We will provide additional updates on this work here. Please continue to share your feedback and provide suggestions at the 
+Inclusive Public Safety Advisory Committee website. Our goal 
 is to achieve as quickly as possible the conditions that enable us to 
-open the Morningside campus gates and ensure a safe environment where 
-everyone feels welcome on our campus. I am confident that we are up to 
-the challenge.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear members of the Columbia community:
-I want to welcome all of you back to campus. As you well know, we begin 
+open the Morningside campus gates and ensure a safe environment where everyone feels welcome on our campus. I am confident that we are up to the challenge.</t>
+  </si>
+  <si>
+    <t>I want to welcome all of you back to campus. As you well know, we begin 
 this spring semester at a moment of significant change in the world and 
-our nation. Institutions succeed at managing such passages when informed 
-by genuine dialogue with people from all backgrounds and experiences, 
-including viewpoints that depart from embedded traditions and 
-orthodoxies. Columbia clearly possesses the capacity to think critically 
+our nation. Institutions succeed at managing such passages when informed by genuine dialogue with people from all backgrounds and experiences, including viewpoints that depart from embedded traditions and orthodoxies. Columbia clearly possesses the capacity to think critically 
 about our institution and its future. This strength is visible in the 
 diversity of our community, the intellectual curiosity on display in our 
-classrooms, and the breadth and depth of academic pursuits unmatched in 
-all of higher education. Our calling is to embrace this moment and its 
+classrooms, and the breadth and depth of academic pursuits unmatched in all of higher education. Our calling is to embrace this moment and its 
 challenges with a feeling of optimism and determination about what we 
 can achieve by working together.
 At the beginning of last semester, I shared my priorities for steadying 
-our community at a time of internal change and uncertainty 
-&lt;https://president.columbia.edu/news/looking-ahead-new-academic-year&gt;. 
-As we embark on this semester, I am committed to continuing our progress 
+our community at a time of internal change and uncertainty. As we embark on this semester, I am committed to continuing our progress 
 on those efforts, grounding all that we do in our dedication to our 
 students and their experience, and embracing the critical work that will 
 ensure our university's success over the years to come.
@@ -704,19 +675,12 @@
 insights, work, and dedication of us all. We must both embrace 
 Columbia's longstanding commitment to the individual pursuit of 
 excellence and recognize that every one of us has a part to play in this 
-important collective endeavor. The time to define our future is now.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York
-</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-I want to wish each of you a very Happy New Year and a warm welcome to 
-our upcoming Spring semester.
+important collective endeavor. The time to define our future is now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to wish each of you a very Happy New Year and a warm welcome to our upcoming Spring semester.
 Throughout the course of this academic year, I have been emphasizing 
-Columbia's mission, the ways we are enriching community engagement, and 
-the steps being taken to safeguard freedom of expression, reject 
+Columbia's mission, the ways we are enriching community engagement, and the steps being taken to safeguard freedom of expression, reject 
 discrimination, and appropriately manage protests and other disruptive 
 activity. Today, as we enter a new year and reflect on this time of 
 global uncertainty, I want to focus on the vital importance of 
@@ -771,100 +735,50 @@
 leave it stronger for future generations.
 I hope you have a good winter break, and I look forward to all we will 
 accomplish in the semester ahead.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
+</t>
   </si>
   <si>
     <t>Dear members of the Columbia community:
 Building on my recent communications, I am writing today to update you 
 on our progress on two of the other priorities I set out for the 
-semester 
-&lt;https://president.columbia.edu/news/update-our-approach-protests-and-demonstrations&gt;—*addressing 
-discrimination and harassment and managing protests and other disruptions*.
+semester addressing discrimination and harassment and managing protests and other disruptions.
 Columbia, as an institution, has long stood as a space for rigorous 
 inquiry, intellectual diversity, and the free exchange of ideas. 
-*Achieving and sustaining this vision requires frameworks and norms that 
+Achieving and sustaining this vision requires frameworks and norms that 
 enable all members of our community to speak and to be heard with 
-dignity and respect*. Columbia's Rules of University Conduct are 
+dignity and respect. Columbia's Rules of University Conduct are 
 designed to provide these crucial guardrails. Although these guardrails 
 were created over 50 years ago, they had been untested at such a scale 
 until the events of the last year. Given this challenge, the effective 
 articulation and implementation of the Rules has been a major focus of 
 the last few months, and we have made important progress in that regard.
-Under the leadership of Professor Greg Wawro, the *Office of Rules 
-Administration has emphasized increased communication and transparency*, 
-including an updates page 
-&lt;https://universitylife.columbia.edu/content/updates-rules-administrator&gt;, 
-a soon-to-be-launched Rules Administrator website, and meetings with 
-student and faculty groups. At the same time, we continue to emphasize a 
-*more effective alignment across the key components of our Rules-based 
-system*, including the Senate Rules Committee, the University Judicial 
-Board, and our delegates and Public Safety team members who manage 
-active demonstrations. The willingness of members of the Columbia 
-community to participate in these efforts is essential for ensuring the 
-confidence of our community. I am deeply grateful for their service.
-Alongside this commitment, the *Office of Institutional Equity (OIE) has 
-implemented new processes* to improve the community's experience of 
-their work, with a particular goal of improving *timely resolution of 
-reports*. OIE's &lt;https://institutionalequity.columbia.edu/&gt; educational 
-programs and trainings are being expanded so that everyone across the 
-University can understand their responsibilities in identifying and 
-eliminating harassment and discrimination. Given the evolving external 
-and internal landscape, *OIE is continuing to refine its processes and 
-programs*, engaging experts and stakeholders across our community as we 
-seek to address concerns about harassment and discrimination while 
-upholding our commitment to free expression and discourse.
-Beyond any formal guardrails, we know that *community norms* have the 
-greatest power to create an environment where disagreement coexists with 
-empathy and compassion, and where ideas and viewpoints are exchanged 
-respectfully without fear of retribution or harassment. While Columbia 
-has a long history of such community norms, last year's experiences, 
-exacerbated by increased social media engagement, have highlighted the 
-need to rebuild this established strength.
+Under the leadership of Professor Greg Wawro, the Office of Rules 
+Administration has emphasized increased communication and transparency, including an updates page, a soon-to-be-launched Rules Administrator website, and meetings with student and faculty groups. At the same time, we continue to emphasize a more effective alignment across the key components of our Rules-based system, including the Senate Rules Committee, the University Judicial Board, and our delegates and Public Safety team members who manage active demonstrations. The willingness of members of the Columbia community to participate in these efforts is essential for ensuring the confidence of our community. I am deeply grateful for their service. Alongside this commitment, the Office of Institutional Equity (OIE) has implemented new processes to improve the community's experience of their work, with a particular goal of improving timely resolution of reports. OIE's educational programs and trainings are being expanded so that everyone across the University can understand their responsibilities in identifying and eliminating harassment and discrimination. Given the evolving external and internal landscape, OIE is continuing to refine its processes and programs, engaging experts and stakeholders across our community as we seek to address concerns about harassment and discrimination while upholding our commitment to free expression and discourse.
+Beyond any formal guardrails, we know that community norms have the 
+greatest power to create an environment where disagreement coexists with empathy and compassion, and where ideas and viewpoints are exchanged respectfully without fear of retribution or harassment. While Columbia has a long history of such community norms, last year's experiences, exacerbated by increased social media engagement, have highlighted the need to rebuild this established strength.
 While organized trainings and updated policies are important, norms are 
 largely driven by the behavior of leaders, both formal and informal, 
-across our community. *Meaningful progress requires deep engagement from 
-student, faculty, and staff leaders* who commit to the work that needs 
-to be done and embrace the impact they can have. The *Student Leadership 
-Engagement Initiative*, which includes over 60 student leaders from 
-across all schools, is one group that exemplifies this effort, as do key 
+across our community. Meaningful progress requires deep engagement from student, faculty, and staff leaders who commit to the work that needs to be done and embrace the impact they can have. The Student Leadership Engagement Initiative, which includes over 60 student leaders from across all schools, is one group that exemplifies this effort, as do key 
 staff advisory groups. Over the next weeks, Provost Olinto and I will be 
-holding f*aculty listening sessions to understand perspectives on 
-several areas, including this critical topic of community leadership*.
+holding faculty listening sessions to understand perspectives on 
+several areas, including this critical topic of community leadership.
 As we head toward the end of a challenging year, I could not believe 
 more strongly that our success depends upon our willingness to come 
 together around a commitment to treating each person with respect and 
 care, thereby upholding the values that have shaped this institution and 
 ensuring that Columbia continues to exemplify the best of what a 
-University can offer.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-Since the start of the semester, I have had the privilege of engaging 
-with many members of our community who care deeply about Columbia and 
-our future. These conversations have highlighted our belief in the role 
+University can offer.</t>
+  </si>
+  <si>
+    <t>Since the start of the semester, I have had the privilege of engaging 
+with many members of our community who care deeply about Columbia and our future. These conversations have highlighted our belief in the role 
 of academic institutions as beacons for reason, resilience, and hope and 
 our shared commitment to nurturing a university where all can thrive, 
 bringing together different voices, fostering understanding and 
 collaboration, and rejecting all forms of discrimination, harassment, or 
 violence.
-In that spirit, I write today with an update on the Campus 
-Collaborative, an initiative that was launched earlier this fall. This 
-effort is designed to harness the ideas, energy, and perspectives of our 
-community—faculty, students, and staff alike—to create an environment 
-where everyone can flourish, both individually and collectively.
-The Campus Collaborative &lt;https://campuscollaborative.columbia.edu/&gt; 
-notified the first set of award recipients last week, funding a series 
-of pilot projects that reflect a wide range of creative approaches to 
-fostering connection across our campuses. From arts initiatives to 
-cross-cultural dialogue, including an expanded Listening Table program, 
-to new methods of engaging with critical contemporary issues, these 
-projects embody the spirit of collaboration that is at the heart of this 
-initiative. With the funding of these projects, we will also be 
+In that spirit, I write today with an update on the Campus Collaborative, an initiative that was launched earlier this fall. This effort is designed to harness the ideas, energy, and perspectives of our community—faculty, students, and staff alike—to create an environment where everyone can flourish, both individually and collectively.
+The Campus Collaborative notified the first set of award recipients last week, funding a series of pilot projects that reflect a wide range of creative approaches to fostering connection across our campuses. From arts initiatives to cross-cultural dialogue, including an expanded Listening Table program, to new methods of engaging with critical contemporary issues, these projects embody the spirit of collaboration that is at the heart of this initiative. With the funding of these projects, we will also be 
 launching the Campus Collaborative Network to bring together awardees 
 and other community members to ensure that we are identifying and 
 addressing the most important opportunities to improve our collective 
@@ -874,16 +788,7 @@
 Even as a primary goal of the Collaborative is to build connections 
 across the University, there is no doubt that our local environments 
 play a critical role in our sense of belonging and community. Thus, the 
-Collaborative has created a dynamic compendium 
-&lt;https://campuscollaborative.columbia.edu/content/resources&gt; of 
-educational, training, and other resources that can support 
-community-building efforts within units, departments, and schools. This 
-resource will continue to grow as we learn from our experience about the 
-most effective approaches to creating an inclusive community, serving as 
-a platform to share current evidence, innovative tools, and best practices.
-As we move forward, we will be highlighting our progress on the Campus 
-Collaborative website. I hope that you will visit the site 
-&lt;https://campuscollaborative.columbia.edu/&gt;, learn more about the 
+Collaborative has created a dynamic compendium of educational, training, and other resources that can support community-building efforts within units, departments, and schools. This resource will continue to grow as we learn from our experience about the most effective approaches to creating an inclusive community, serving as a platform to share current evidence, innovative tools, and best practices. As we move forward, we will be highlighting our progress on the Campus Collaborative website. I hope that you will visit the site, learn more about the 
 initiative, and consider how you can contribute. We will continue to 
 accept applications for new pilot projects on a rolling basis and 
 welcome suggestions for resources that can be included in the compendium.
@@ -891,19 +796,11 @@
 of our Columbia community. I look forward to working alongside all of 
 you as we continue to innovate, share ideas, and build connections that 
 will shape the future of our institution. Together, we can create a 
-stronger, more inclusive Columbia for generations to come.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-At the beginning of this semester, I set out several priorities for this 
-academic year 
-&lt;https://president.columbia.edu/news/looking-ahead-new-academic-year&gt;, 
-first among them affirming Columbia's mission and placing our mission 
-and principles at the center of our decision-making. Over the final 
-weeks of the semester, we will be sharing updates on these priorities, 
+stronger, more inclusive Columbia for generations to come.</t>
+  </si>
+  <si>
+    <t>At the beginning of this semester, I set out several priorities for this 
+academic year first among them affirming Columbia's mission and placing our mission and principles at the center of our decision-making. Over the final weeks of the semester, we will be sharing updates on these priorities, 
 reflecting on the progress, challenges, and road ahead. Today, I am 
 writing to engage you in what it means for our community to actively 
 embody our mission and principles at this turbulent time.
@@ -926,11 +823,8 @@
 vibrant community life that draws on the vitality of the remarkable city 
 around us. So many faculty stay at Columbia because of their students 
 and so many alumni tell me how Columbia changed their life trajectory. 
-As we look forward, I believe we must deepen this commitment, asking how 
-we can strengthen the connections between students and faculty, ensure 
-that students have the resources needed to succeed, and create an 
-environment, both in and outside the classroom, where everyone can grow 
-and thrive.
+As we look forward, I believe we must deepen this commitment, asking how we can strengthen the connections between students and faculty, ensure that students have the resources needed to succeed, and create an 
+environment, both in and outside the classroom, where everyone can grow and thrive.
 Columbia has a storied tradition of embracing intellectual debate. The 
 daily debates that occur in and beyond our classrooms have long brought 
 the most brilliant minds to study and teach at Columbia, joining a 
@@ -949,21 +843,7 @@
 also must redouble our commitment to the norms and guardrails that 
 protect free expression and enable a vibrant, diverse community to 
 thrive. We have made substantial progress this year in the fair and 
-effective application of our Rules of University Conduct 
-&lt;https://universitypolicies.columbia.edu/content/rules-university-conduct&gt; 
-and our policies, but our work must continue. Too many members of our 
-community have felt unheard or unseen as they struggle with immensely 
-distressing events on our campus and in the wider world. We must stand 
-up as a community to repudiate antisemitism, discrimination, and 
-harassment of any kind. No one here should feel threatened or fear for 
-their wellbeing, and it should go without saying that we have zero 
-tolerance for anyone promoting or calling for terror or violence. Over 
-the last months, I have also been moved by the many times when our 
-community has responded to the pain or vulnerability of others with the 
-empathy and humility required to truly support those in need. We must 
-continue to learn from these experiences, strengthen our commitment to 
-addressing discrimination of any form, and draw on these experiences to 
-build a stronger, wiser, and more resilient community.
+effective application of our Rules of University Conduct and our policies, but our work must continue. Too many members of our community have felt unheard or unseen as they struggle with immensely distressing events on our campus and in the wider world. We must stand up as a community to repudiate antisemitism, discrimination, and harassment of any kind. No one here should feel threatened or fear for their wellbeing, and it should go without saying that we have zero tolerance for anyone promoting or calling for terror or violence. Over the last months, I have also been moved by the many times when our community has responded to the pain or vulnerability of others with the empathy and humility required to truly support those in need. We must continue to learn from these experiences, strengthen our commitment to addressing discrimination of any form, and draw on these experiences to build a stronger, wiser, and more resilient community.
 We have navigated many difficult and disruptive events throughout 
 Columbia's long history, including, and perhaps especially, over the 
 last year. Undoubtedly, we will face new challenges ahead. Truly 
@@ -974,58 +854,15 @@
 preserve the open intellectual discourse and rigorous research that 
 define what Columbia means to the City, the nation, and the world.  I 
 have every confidence that we have the will, the ability, and the 
-strength to fulfill this commitment.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-Presidential elections are moments of civic engagement that shape the 
-country's policy agenda and political direction for the coming four 
-years. Historically in this country, elections have had consequences for 
-the scale of government; economic, tax and regulatory policy; foreign 
-policy ambitions; and how the nation will address equity and justice, 
-among other issues.
-We are living in unusual times. Many Columbia students, including 
-undergraduates who may be casting their first votes, have only 
-experienced presidential elections as national referendums that can feel 
-as if they have existential significance. The intensity of political 
-disagreement and the acrimony it can cause are unfortunate on many 
-levels. The nation and our communities will be better off when we are 
-able to move beyond this divisiveness to find common ground.
-In this political context, I urge you to keep in mind that civic 
-participation is an important part of life in a democracy and consistent 
-with Columbia's commitment to free expression and dialogue. So, too, is 
-tolerance of different views, including those with which we may strongly 
-disagree. Over the University's long history, and through the course of 
-many political changes, Columbia's academic mission of teaching, 
-advancing knowledge, and educating new generations of leaders has been a 
-source of strength. That will remain so during the weeks, months, and 
-years ahead.
-My highest priorities for the University this fall have been to 
-strengthen our community, enhance the student experience on campus, and 
-build our capacity for open and respectful discussion and dialogue 
-consistent with our values and mission. I deeply appreciate that so many 
-of you have joined in this effort. Next week's election will be another 
-opportunity for us to draw on the strengths of our community and to 
-learn from each other as we navigate whatever outcome occurs. I am 
-confident that we have the ability to do so.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear members of the Columbia community:
-Over the many years that I have spent studying and practicing medicine, 
-I have come to believe that excellence requires both a focus on 
+strength to fulfill this commitment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over the many years that I have spent studying and practicing medicine, I have come to believe that excellence requires both a focus on 
 achieving the best possible outcomes for each person and on doing our 
 best to support their individual journey through complicated and 
 challenging times. I write to you today recognizing the understandable 
 concerns many of you have about the uncertain social and political 
-environment we may face on campus over the next weeks. I want to assure 
-you that the University's leadership is working together to prepare for 
-this period and to support our community.
+environment we may face on campus over the next weeks. I want to assure you that the University's leadership is working together to prepare for this period and to support our community.
 I appreciate that, across our diverse community, individuals and groups 
 have had very different experiences over the past year. The terror 
 attack on October 7 and the ensuing war have affected us all, some more 
@@ -1047,14 +884,7 @@
 While all of us benefit from the support of our classmates and 
 colleagues, I encourage those who may need additional help to seek 
 counseling and other resources during this time. Please reach out to 
-Columbia Health &lt;https://www.health.columbia.edu/&gt; (Morningside, 
-Manhattanville, and Teachers College; in-person, telehealth, and virtual 
-options) or Student Health on Haven 
-&lt;https://www.studenthealth.cuimc.columbia.edu/&gt; (CUIMC students; 
-in-person and telehealth). For faculty and staff, mental health 
-resources are available here 
-&lt;https://humanresources.columbia.edu/mental-health&gt;. University Life 
-&lt;https://universitylife.columbia.edu/well-being&gt; provides additional 
+Columbia Health (Morningside, Manhattanville, and Teachers College; in-person, telehealth, and virtual options) or Student Health on Haven (CUIMC students; in-person and telehealth). For faculty and staff, mental health resources are available here. University Life provides additional 
 wellbeing resources and tips. Individual schools also offer support for 
 their students, staff and faculty.
 An extraordinary attribute of an academic community devoted to teaching 
@@ -1062,50 +892,16 @@
 past, to make this journey together, and to become a stronger community 
 as a result. I have every confidence that Columbia is poised to 
 demonstrate our leadership in this regard.
-All my best,
-Katrina Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear members of the Columbia community:
-I am writing to update you on our current situation on campus, our 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am writing to update you on our current situation on campus, our 
 understanding of what different groups are planning given the 
 significance of the week ahead, and our preparations to support you and 
 the Columbia community.
-As I expressed in my message last week 
-&lt;https://president.columbia.edu/news/supporting-our-community&gt;, we 
-anticipated and have been preparing for a period of uncertainty in the 
-coming days. Over the last few days, and particularly the last 24 hours, 
-there has been rapidly increasing evidence that the Morningside campus 
-is a major focus for protest and other activity. We have several student 
-groups planning for special events and non-violent protests and are 
-working diligently to support those plans with public safety and 
-delegate support. At the same time, we have also learned and had 
-evidence of plans of groups not affiliated with Columbia choosing to 
-come to our Morningside campus for activities that raise concern about 
-the potential for violence. We understand that there has been a call for 
-a walkout as part of a larger protest effort across New York City. This 
-walkout was not registered through the process established by the 
-Guidelines to the Rules of University Conduct and thus is not sanctioned 
-by the University Senate or the University administration. We continue 
-to implement public safety measures to plan for every eventuality. We 
-take those concerns with extreme seriousness.
+As I expressed in my message last week we anticipated and have been preparing for a period of uncertainty in the coming days. Over the last few days, and particularly the last 24 hours, there has been rapidly increasing evidence that the Morningside campus is a major focus for protest and other activity. We have several student groups planning for special events and non-violent protests and are working diligently to support those plans with public safety and delegate support. At the same time, we have also learned and had evidence of plans of groups not affiliated with Columbia choosing to come to our Morningside campus for activities that raise concern about the potential for violence. We understand that there has been a call for a walkout as part of a larger protest effort across New York City. This walkout was not registered through the process established by the Guidelines to the Rules of University Conduct and thus is not sanctioned by the University Senate or the University administration. We continue to implement public safety measures to plan for every eventuality. We take those concerns with extreme seriousness.
 Because of this information and in line with our responsibility for the 
-safety of our campus community, we are taking several immediate steps to 
-ensure that our campus can continue to carry out our academic mission, 
-particularly in the classroom. First, for today and tomorrow (October 6 
-- 7) and possibly later into the week, we are no longer accepting the QR 
-codes generated when guest access to the Morningside campus is requested 
-and will be working closely with leadership across the schools and 
-programs to determine where guest access is critical for our academic 
-mission. We are also working on revising the automated system so that it 
-can be used again. Anyone who is not a current employee or student is 
-considered guest for this purpose. We are also working to develop 
-approaches for student groups who were hoping to have meetings with 
-guests on Morningside campus at other locations and to provide support 
-for all our students to see their family and friends at this challenging 
-time.
+safety of our campus community, we are taking several immediate steps to ensure that our campus can continue to carry out our academic mission, particularly in the classroom. First, for today and tomorrow (October 6- 7) and possibly later into the week, we are no longer accepting the QR codes generated when guest access to the Morningside campus is requested and will be working closely with leadership across the schools and programs to determine where guest access is critical for our academic mission. We are also working on revising the automated system so that it can be used again. Anyone who is not a current employee or student is considered guest for this purpose. We are also working to develop approaches for student groups who were hoping to have meetings with guests on Morningside campus at other locations and to provide support for all our students to see their family and friends at this challenging time.
 Second, we will be increasing the public safety presence across campus 
 for the next three days. We are all eager to get back to an environment 
 where that is not needed and appreciate the challenges that widespread 
@@ -1130,7 +926,6 @@
 restricted gate access status for the next three days. Restricted access 
 means that some gates will not be available. Information about gate 
 access is available at the Public Safety Morningside Campus Access page 
-&lt;https://publicsafety.columbia.edu/content/morningside-campus-access-updates&gt;. 
 We will take the necessary steps to respond to these developments while 
 working to support the student group special events that are currently 
 scheduled, as well as non-violent demonstrations that have been sent 
@@ -1145,15 +940,10 @@
 partners across the city and the state. None of these are easy decisions 
 and we will continue to ground every decision in our mission and our 
 principles and expand our engagement and dialogue as we move forward.
-All my best,
-Katrina Armstrong
-Interim President
-Columbia University in the City of New York
 </t>
   </si>
   <si>
-    <t>Dear members of the Columbia community:
-I am writing to share with you how we are thinking about access to the 
+    <t xml:space="preserve">I am writing to share with you how we are thinking about access to the 
 Morningside campus over the upcoming weeks. The concerns we are 
 balancing go beyond having to display a Columbia ID to gain entry, or 
 the time consumed by waiting in line at our campus gates, though in no 
@@ -1172,18 +962,7 @@
 and recognize as foundational to our distinctive contributions to society.
 At the same time, I have heard from many students, faculty, and staff, 
 in discussions both formal and informal, about the importance of having 
-a campus environment that enables the dialogue, connection, and empathy 
-we need to learn from and move beyond the events of the past year. Many 
-of you have expressed your gratitude for the intimate atmosphere of our 
-campus this September and the opportunity to immerse yourselves in your 
-academic work and all the things you cherish about this special 
-community. Many others, including those beyond our campus, have 
-appreciated the need for our community to take the necessary time to be 
-together, to heal and move forward. Concerns about the uncertainty of 
-the political environment over the next weeks have been central to many 
-of these conversations. Many people have also highlighted how 
-disruptions on our campus can affect our Morningside Heights and other 
-community neighbors.
+a campus environment that enables the dialogue, connection, and empathy we need to learn from and move beyond the events of the past year. Many of you have expressed your gratitude for the intimate atmosphere of our campus this September and the opportunity to immerse yourselves in your academic work and all the things you cherish about this special community. Many others, including those beyond our campus, have appreciated the need for our community to take the necessary time to be together, to heal and move forward. Concerns about the uncertainty of the political environment over the next weeks have been central to many of these conversations. Many people have also highlighted how disruptions on our campus can affect our Morningside Heights and other community neighbors.
 Given these conversations, I have decided to continue our current 
 restrictions on Morningside access for the time being, while moving 
 thoughtfully and deliberately toward a fully reopened campus, a 
@@ -1205,21 +984,14 @@
   * The security presence on campus will continue to be adjusted as
     appropriate.
 Over the last weeks I have had the great pleasure of speaking with many 
-members of our community about the history of the Morningside campus and 
-the robust, ongoing dialogue about how best to align that campus with 
-our values and our aspirations. I look forward to continuing those 
+members of our community about the history of the Morningside campus and the robust, ongoing dialogue about how best to align that campus with our values and our aspirations. I look forward to continuing those 
 discussions as we work to ensure that our campus spaces advance our 
 academic mission, strengthen our engagement with the City of New York, 
 and create an environment supporting individual and collective wellbeing.
-All my best,
-Katrina Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-Throughout the events of the past year, our Columbia community has been 
-engaged in an ongoing discussion about how the University can best 
+</t>
+  </si>
+  <si>
+    <t>Throughout the events of the past year, our Columbia community has been engaged in an ongoing discussion about how the University can best 
 fulfill its academic mission of teaching, learning, and research while 
 creating and sustaining an environment that enables free expression, 
 rigorous debate, and open dialogue. Similar discussions have taken place 
@@ -1246,8 +1018,7 @@
 announced in the near future.
 We are fortunate to have scholars of Dean Abebe's and Professor 
 Mazower's stature and expertise leading this critical work for Columbia. 
-Once the Advisory Committee is formed, the Co-Chairs plan to commence a 
-consultative process through which they will engage our faculty, 
+Once the Advisory Committee is formed, the Co-Chairs plan to commence a consultative process through which they will engage our faculty, 
 students, and staff, as well as the University Senate and other relevant 
 groups within our community. I am confident that Dean Abebe and 
 Professor Mazower and the Advisory Committee will lead a rigorous and 
@@ -1261,14 +1032,10 @@
 as it will help to guide the ways in which we protect and enable free 
 expression and vigorous debate in our community. I hope that you will 
 take the opportunity to engage in the Advisory Committee's consultative 
-process and support its service on behalf of Columbia.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-As I shared with you several weeks ago, one of my priorities for this 
+process and support its service on behalf of Columbia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As I shared with you several weeks ago, one of my priorities for this 
 year is to strengthen engagement across our University, including the 
 meaningful dialogue of leaders at all levels with the many groups and 
 communities that make up this vibrant institution. Such engagement is 
@@ -1304,12 +1071,10 @@
 Engagement over the last weeks has helped us to see what we need to set 
 in motion to address key issues for students and student groups in the 
 long term, as well as steps that can be taken now to address immediate 
-concerns. Our implementation of these ideas is informed and supported by 
-the experience and operational expertise of the central and school 
+concerns. Our implementation of these ideas is informed and supported by the experience and operational expertise of the central and school 
 teams. A few examples of the steps we are taking that result from this 
 engagement process include:
   * We are launching a University International Student Hardship Fund
-    &lt;https://sfs.columbia.edu/content/university-international-student-hardship-fund&gt;
     for students experiencing financial hardship due to natural
     disasters, humanitarian crises, armed conflict, and other crises.
     This fund will support living expenses for degree-seeking students.
@@ -1336,15 +1101,7 @@
 impressed by the deep commitment of these groups to advancing engagement 
 across the University, whether through school-level discussions, small 
 group meetings, or developing innovative new ideas like the Listening 
-Tables &lt;https://urldefense.proofpoint.com/v2/url?u=https-3A__www.trustcollaboratory.org_listening-2Dtables&amp;d=DwIDaQ&amp;c=009klHSCxuh5AI1vNQzSO0KGjl4nbi2Q0M1QLJX9BeE&amp;r=_sS6e46Spcl5nvpuIffnet3bGSmYljzZebuBoNgTiZE&amp;m=1_zxx-UBgotbj6lUxlA1WdkbcqsjA9qQT4QifD7wYbPymS_cjRYYD4hDg1kDW65C&amp;s=fXEEEiBW_AYD-iqvkxVndfdGmjDFjnWt2iTvi6gqNVw&amp;e= &gt; that are 
-being hosted by the Trust Collaboratory at Columbia to promote listening 
-and dialogue on campus. Next week we will be sharing the next steps in 
-the Campus Climate Collaborative 
-&lt;https://president.columbia.edu/news/introducing-campus-climate-collaborative&gt;, 
-including ways to participate, access to shared resources and 
-opportunities for programmatic support. I am grateful to Dennis Mitchell 
-for his dedication to that effort and his continued leadership in this 
-critical area.
+Tables that are being hosted by the Trust Collaboratory at Columbia to promote listening and dialogue on campus. Next week we will be sharing the next steps in the Campus Climate Collaborative, including ways to participate, access to shared resources and opportunities for programmatic support. I am grateful to Dennis Mitchell for his dedication to that effort and his continued leadership in this critical area.
 I have absolutely no doubt that the strength of our University lies with 
 the extraordinary people—students, faculty, staff—who bring Columbia to 
 life every day. Each person I meet tells me that is what brought them to 
@@ -1353,28 +1110,11 @@
 our mission—and creates the unique and dynamic environment of our 
 University.
 Please don't hesitate to reach out.
-All my best,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-Two weeks ago, I wrote to all of you 
-&lt;https://president.columbia.edu/news/looking-ahead-new-academic-year&gt; to 
-affirm our mission and our values and lay out my priorities for the 
-coming academic year. I said I would continue to share new developments 
-on those priorities as often as I could. We have already announced a new 
-Office of Institutional Equity 
-&lt;https://institutionalequity.columbia.edu/&gt; and launched the Campus 
-Climate Collaborative 
-&lt;https://president.columbia.edu/news/introducing-campus-climate-collaborative&gt;, 
-both of which will add to our ongoing efforts to build and sustain a 
-community at Columbia where everyone can thrive. Today, I would like to 
-focus on our approach to protests and demonstrations, which is an 
-essential part of how we advance our educational and research mission, 
-safeguard free expression and open debate, and ensure a safe, respectful 
-campus environment for our community.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Two weeks ago, I wrote to all of you to affirm our mission and our values and lay out my priorities for the coming academic year. I said I would continue to share new developments on those priorities as often as I could. We have already announced a new Office of Institutional Equity  and launched the Campus Climate Collaborative, both of which will add to our ongoing efforts to build and sustain a community at Columbia where everyone can thrive. Today, I would like to focus on our approach to protests and demonstrations, which is an essential part of how we advance our educational and research mission, safeguard free expression and open debate, and ensure a safe, respectful campus environment for our community.
 I would like to make it clear, up front, that I support the right to 
 free expression at Columbia. I believe deeply in the values of free 
 speech, open inquiry, and rigorous debate. But those rights cannot come 
@@ -1389,17 +1129,8 @@
 in the free expression of opinion in protests and demonstrations, as 
 long as these do not substantially disrupt the University's academic 
 activities.” I am grateful to the University Senate and its Rules of 
-University Conduct Committee 
-&lt;https://senate.columbia.edu/committees/rules&gt; for their efforts. I 
-encourage everyone to visit their website for updated information 
-&lt;https://senate.columbia.edu/content/guidelines-rules-university-conduct&gt; 
-and answers to frequently asked questions 
-&lt;https://senate.columbia.edu/content/guidelines-rules-university-conduct-faqs&gt;, 
-including how to report alleged Rules violations, policies on 
-encampments, and the obligation to unmask and identify oneself when 
-appropriately asked.
-It is the responsibility of our administration to make sure these rules 
-are implemented thoughtfully, fairly, and efficiently. The 
+University Conduct Committee for their efforts. I encourage everyone to visit their website for updated information and answers to frequently asked questions, including how to report alleged Rules violations, policies on encampments, and the obligation to unmask and identify oneself when 
+appropriately asked. It is the responsibility of our administration to make sure these rules are implemented thoughtfully, fairly, and efficiently. The 
 implementation process includes multiple components including 
 disseminating information about the Guidelines and the Rules, ensuring 
 delegate and public safety resources are available as needed, and 
@@ -1423,7 +1154,6 @@
     Rules at the time of protests or other events. University delegates
     support the University's commitment to freedom of expression while
     identifying potential violations to the Rules of University Conduct
-    &lt;https://universitypolicies.columbia.edu/content/rules-university-conduct&gt;.
   * Based upon feedback from the listening sessions conducted by the
     Inclusive Public Safety Advisory Committee, I have asked the Public
     Safety leadership to advance our efforts to create a
@@ -1434,10 +1164,8 @@
     importance of ongoing feedback and evaluation of our public safety
     efforts. Please continue to share your thoughts with us at the
     Inclusive Public Safety Advisory Committee website
-    &lt;https://universitylife.columbia.edu/inclusive-public-safety&gt;.
 Consistent and effective implementation of our rules requires a rigorous 
-framework for how we respond to any situation where concerns arise about 
-the impact of an event on our academic mission or the safety of our 
+framework for how we respond to any situation where concerns arise about the impact of an event on our academic mission or the safety of our 
 community. We have looked to the best practices from decision sciences 
 and social sciences to guide us in a framework for assessment, 
 decision-making, and response that enables an integrated approach to 
@@ -1450,40 +1178,24 @@
 inform our dynamic assessment effort that examines the potential impact 
 of any event on our academic—teaching, learning, and research—mission, 
 the physical safety of our community members, and our surrounding 
-neighborhoods. Our processes are committed to a thoughtful consideration 
-of a range of judicious and careful approaches for managing response 
-according to our values and mission. We will continue to refine this 
-framework and processes as we move forward by learning from each 
+neighborhoods. Our processes are committed to a thoughtful consideration of a range of judicious and careful approaches for managing response according to our values and mission. We will continue to refine this framework and processes as we move forward by learning from each 
 experience, engagement with our faculty, students and staff, and 
 approaches used by peer institutions.
 Over the last few days, I have seen the University come alive with new 
 and returning students and faculty, alongside the staff who make it all 
 possible. The energy and engagement as I walk around campus is such a 
-great reminder of how we all come together to build the campus community 
-that every Columbian deserves. This includes supporting the Rules of 
-University Conduct that serve our mission to teach, create, and advance 
-knowledge and the values that underpin it. I look forward to working 
-with all of you on these next steps.
-All my best,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>To Our Fantastic Columbia Students:
-I have spent the last few weeks getting to know many of you during 
+great reminder of how we all come together to build the campus community that every Columbian deserves. This includes supporting the Rules of University Conduct that serve our mission to teach, create, and advance knowledge and the values that underpin it. I look forward to working with all of you on these next steps.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have spent the last few weeks getting to know many of you during 
 orientation. Building upon my great conversations with the NSOP 
 leadership, I attended a barbeque with resident advisors and orientation 
 leaders, welcomed members of the football team, greeted first-years 
 moving into the residence halls, met with members of the student 
 government, gave out backpacks to SEAS students, joined the academic 
 resources fair, and crashed welcome events for incoming graduate students.
-One theme has come up over and over again in these conversations. When I 
-ask our students what they love most about Columbia, they talk about how 
-Columbia embraces each of them as an individual and understands the 
-unique role that each person plays in creating the larger University 
-community. And in doing so, Columbia empowers each of its members to be 
-freer, braver, and more themselves.
+One theme has come up over and over again in these conversations. When I ask our students what they love most about Columbia, they talk about how Columbia embraces each of them as an individual and understands the unique role that each person plays in creating the larger University community. And in doing so, Columbia empowers each of its members to be freer, braver, and more themselves.
 Your peers told me that the experience of being a Columbian, of living 
 and learning here with our brilliant scholars in this diverse and 
 incredible city, has transformed the way they see themselves and what 
@@ -1506,8 +1218,7 @@
 As I welcome you to the start of this new academic year, I know that we 
 have work to do to stay true to our mission to impart, create, and 
 advance knowledge and build the campus climate you all deserve, where 
-everyone can learn and thrive. As I said in my Convocation Address 
-&lt;https://president.columbia.edu/content/2024-convocation-address&gt; to the 
+everyone can learn and thrive. As I said in my Convocation Address to the 
 newest undergraduates, “Everyone needs to feel engaged, that their 
 voices matter, and that they belong here.” A lot of people who care 
 deeply about this institution have been doing this work for some time, 
@@ -1522,19 +1233,12 @@
 Columbia experience. My approach to supporting that experience must be 
 grounded in conversations I have and will continue to have with you and 
 your peers. I want to make sure that this University is a place that 
-embraces you, educates you, and pushes you to make the most of your time 
-here. I want everyone to feel what I have heard over the last weeks from 
-so many students—that being a Columbian will transform your life. You 
-deserve nothing less.
+embraces you, educates you, and pushes you to make the most of your time here. I want everyone to feel what I have heard over the last weeks from so many students—that being a Columbian will transform your life. You deserve nothing less.
 Again, welcome and welcome back. I look forward to seeing you.
-All my best,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-Last Friday, I called on all of us to remember that our mission is to 
+</t>
+  </si>
+  <si>
+    <t>Last Friday, I called on all of us to remember that our mission is to 
 teach, create, and advance knowledge. I said that in doing so we must 
 affirm our values and principles to guide decision-making, to engage 
 across our community, and to address discrimination and harassment.
@@ -1588,19 +1292,13 @@
 environment.
 Over the last two weeks, I have met so many Columbians who believe 
 deeply in our values and our mission and want to do all they can to 
-improve the campus climate for everyone. Many of them have been hard at 
-work on this for some time, and for that, I am very grateful. As we work 
+improve the campus climate for everyone. Many of them have been hard at work on this for some time, and for that, I am very grateful. As we work 
 to assemble the right processes, groups, and partnerships for this 
 effort, I look forward to continuing to get your feedback and to sharing 
-updates as they develop.
-All my best,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-It has been wonderful to connect and reconnect with so many of you on 
+updates as they develop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It has been wonderful to connect and reconnect with so many of you on 
 campus over the past week, as we celebrate the arrival of our new 
 students and the return of our academic community. As the new year 
 unfolds, I am looking forward to working with each of you to fulfill the 
@@ -1612,82 +1310,89 @@
 people are eager to become involved and I am deeply grateful for your 
 willingness to engage in our collective efforts on behalf of Columbia.
 To foster effective governance and collaboration, I have brought 
-together an *Executive Committee* comprised of deans, senior 
+together an Executive Committee comprised of deans, senior 
 administrators, and special advisors. This group will partner with me 
 regularly to advance the University's mission. Additionally, I will 
-convene a *President's Cabinet*, including members of the Executive 
+convene a President's Cabinet, including members of the Executive 
 Committee and other leaders whose work spans the University, to 
 facilitate broader consultation and coordination.
 Central to our endeavors is robust and deep engagement with our faculty, 
 who are the heart of our academic community. I am pleased to announce 
-that *Costis Maglaras*, Dean of Columbia Business School, will chair the 
-Council of Deans, with *Amy Hungerford*, Executive Vice President and 
-Dean of the Faculty of Arts and Sciences, and *Shih-Fu Chang*, Dean of 
+that Costis Maglaras, Dean of Columbia Business School, will chair the 
+Council of Deans, with Amy Hungerford, Executive Vice President and 
+Dean of the Faculty of Arts and Sciences, and Shih-Fu Chang, Dean of 
 The Fu Foundation School of Engineering and Applied Science, serving as 
-co-chairs. The *Council of Deans*, which includes all of the deans from 
+co-chairs. The Council of Deans, which includes all of the deans from 
 our 17 schools, will continue to play a crucial role in shaping our 
-academic strategies. In tandem, *Provost Angela Olinto* has assembled a 
-*Faculty Leadership Council* from the Morningside and Manhattanville 
+academic strategies. In tandem, Provost Angela Olinto has assembled a 
+Faculty Leadership Council from the Morningside and Manhattanville 
 campuses, alongside a similar group at the Columbia University Irving 
 Medical Center (CUIMC). These councils will provide invaluable guidance, 
-feedback, and perspectives. *Sarah Cole*, Dean of the School of the 
-Arts, will also coordinate a President's *advisory group of 
-faculty**across the University*, ensuring that a broad spectrum of 
+feedback, and perspectives. Sarah Cole, Dean of the School of the 
+Arts, will also coordinate a President's advisory group of 
+faculty across the University, ensuring that a broad spectrum of 
 voices and expertise informs our thinking and decisions.
 To further our commitment to fostering an inclusive environment, I am 
-pleased to announce that *Dennis Mitchell* will serve as my *Senior 
-Advisor for Inclusion and Belonging*. Dennis will extend his impactful 
+pleased to announce that Dennis Mitchell will serve as my Senior 
+Advisor for Inclusion and Belonging. Dennis will extend his impactful 
 work as Senior Vice Provost for Faculty Advancement across the 
 University, and will maintain his faculty appointment at the College of 
 Dental Medicine. We are deeply appreciative of Dennis's over 30 years of 
 dedicated service, including his leadership of the Office of University 
 Life.
-*Melanie Bernitz*, Senior Vice President for Columbia Health, will step 
+Melanie Bernitz, Senior Vice President for Columbia Health, will step 
 into the role of Interim Executive Vice President for University Life. 
-Melanie has long been a Columbia citizen and her unwavering commitment 
-to student health and wellbeing make her an excellent fit for this role.
-*Shailagh Murray*, Executive Vice President for Public Affairs, has been 
+Melanie has long been a Columbia citizen and her unwavering commitment to student health and wellbeing make her an excellent fit for this role.
+Shailagh Murray, Executive Vice President for Public Affairs, has been 
 on leave since the end of the spring semester due to a family medical 
 emergency. She recently informed us that she will not return to her EVP 
 role. We extend our heartfelt gratitude for her leadership and 
 dedication. She will continue in an advisory role this fall.
-I am pleased to announce *Franz Paasche* (Columbia Law '87) is joining 
+I am pleased to announce Franz Paasche (Columbia Law '87) is joining 
 my leadership team as our new Executive Vice President for Public 
-Affairs and Communications 
-&lt;https://communications.news.columbia.edu/directory/franz-paasche&gt;. 
-Franz's exceptional expertise and deep experience make him a perfect 
-choice for leading our Public Affairs and Government and Community 
-Affairs teams. We are confident in his ability to help guide us through 
-this pivotal period. I hope you will join me in welcoming Franz back to 
-Columbia. I also wish to express my deep appreciation to *Ben Chang*, 
-Vice President for Communications, for his steadfast leadership during 
-this transition. His dedication and support have been invaluable, and I 
-am thrilled that he will continue to serve as a key member of our team.
-As we step forward into the upcoming academic year, our newly structured 
-leadership team is prepared and committed to strengthening and 
-furthering Columbia's mission of advancing knowledge, fostering 
-innovation, and promoting an inclusive community where every member can 
-thrive. Please join us in approaching the new year with renewed energy 
-and a shared commitment to fulfilling the incredible potential of this 
-great University.
-Sincerely,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>Dear fellow members of the Columbia community:
-As the start of the new academic year approaches, I want to express how 
+Affairs and Communications. Franz's exceptional expertise and deep experience make him a perfect choice for leading our Public Affairs and Government and Community Affairs teams. We are confident in his ability to help guide us through this pivotal period. I hope you will join me in welcoming Franz back to Columbia. I also wish to express my deep appreciation to Ben Chang, Vice President for Communications, for his steadfast leadership during this transition. His dedication and support have been invaluable, and I am thrilled that he will continue to serve as a key member of our team.
+As we step forward into the upcoming academic year, our newly structured leadership team is prepared and committed to strengthening and furthering Columbia's mission of advancing knowledge, fostering 
+innovation, and promoting an inclusive community where every member can thrive. Please join us in approaching the new year with renewed energy and a shared commitment to fulfilling the incredible potential of this great University.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am deeply honored to be called to serve as Interim President of our
+beloved institution. This role comes at a pivotal moment for Columbia, and
+I am excited and humbled by the opportunity to contribute to our collective journey. With profound respect for Columbia's storied history and an unwavering commitment to its future, I look forward to working with you to achieve our shared goals.
+Challenging times present both the opportunity and the responsibility for
+serious leadership to emerge from every group and individual within a
+community. This is such a time at Columbia. As I step into this role, I am
+acutely aware of the trials the University has faced over the past year. We
+should neither understate their significance, nor allow them to define who
+we are and what we will become. The familiar excitement and promise of a
+new academic year are informed this year by the presence of change and
+continuing concerns, but also by the immense opportunity to look forward, to join together for the laudable mission we are here to serve, and to become our best selves individually and institutionally. Never has it been more important to train leaders capable of elevating society and addressing the complexity of modern life. Columbia University has a long history of meeting the moment, and I have faith that we will do so once again. I ask each of you to join me in this critically important work fueled by the enthusiasm for what we can accomplish together. Through our collective effort, I am confident we will succeed.
+Much of this work will fall to the Columbia faculty. You are the ultimate
+keepers of the institution's values and the stewards of its long and proud
+history. The habit of critical thinking and humility that gives birth to
+tolerance of contrary points of view is the most essential lesson taught in
+Columbia's classrooms and the intellectual common ground that unifies the many scholarly pursuits found across our campuses. Physicians learn this philosophical approach quickly as it can often be the difference between life and death. My leadership of Columbia University Irving Medical Center (CUIMC) has been grounded in consistent engagement with the entire faculty across all four schools, and that will again be the case during my time as your Interim University President.
+I assume this role able to stand on the shoulders of our two most recent
+presidents, Minouche Shafik and Lee C. Bollinger, whose dedication to
+Columbia is boundless, and I take comfort in knowing they will be available to me and to Columbia going forward. The University exists because of the love for the institution expressed and the contributions made by countless talented individuals over many decades, particularly our faithful alumni. First among these, in my experience, is P. Roy Vagelos, a visionary leader and supremely generous benefactor, whose friendship I have relied on throughout my time at Columbia and whom I must recognize and thank here.
+I have been privileged to spend my professional life at the greatest
+research universities in the United States, serving as a teacher,
+researcher, attending physician, department chair, administrative leader,
+dean, and, most recently, head of CUIMC, one of the nation's greatest
+academic medical centers. I fully appreciate the profound responsibility of
+meeting the needs of the many constituencies that make Columbia University the renowned leader in higher education that it is. With optimism and resolve, let us move forward together, embracing the opportunity to renew our vision and strengthen our community.
+</t>
+  </si>
+  <si>
+    <t>As the start of the new academic year approaches, I want to express how 
 much I am looking forward to welcoming new and returning students, 
 faculty, and staff to our campuses. I also wanted to take the 
 opportunity to provide further insight into how I am approaching the 
 role of interim president and to share some important updates that 
 involve all of us.
 Over the past several days, I have had the opportunity to meet so many 
-of the wonderful members of our campus community–including members of 
-the A&amp;S Policy and Planning Committee, University Senators, leaders of 
-the New Student Orientation Program (NSOP), resident advisors, incoming 
-students, and dedicated facilities and operations team members 
+of the wonderful members of our campus community–including members of the A&amp;S Policy and Planning Committee, University Senators, leaders of 
+the New Student Orientation Program (NSOP), resident advisors, incoming students, and dedicated facilities and operations team members 
 (including the beloved Chef Mike). While many of my conversations have 
 focused on our opportunity to move forward in new ways, I have also 
 heard people's thoughts about the impact of the prior year and the need 
@@ -1702,18 +1407,14 @@
 preeminence far into the future. I am deeply committed to learning more 
 from our community about the best approaches to that work and will be 
 sharing more about what I learn in the weeks to come.
-Our first priority must be to *affirm our values and principles so that 
-they can guide our decision-making*. This is complicated, of course, and 
+Our first priority must be to affirm our values and principles so that 
+they can guide our decision-making. This is complicated, of course, and 
 there are many ways to understand what we do and why we do. But in all 
 cases, the central mission of this University is to teach, create, and 
-advance knowledge. Our mission is grounded in a fundamental commitment 
-to free expression, open inquiry, and generous debate; it requires an 
-environment of inclusive pluralism where all our community members can 
-thrive. Violence, intimidation, discrimination, bullying, and any 
-behaviors that prevent teaching, learning, or research are antithetical 
+advance knowledge. Our mission is grounded in a fundamental commitment to free expression, open inquiry, and generous debate; it requires an environment of inclusive pluralism where all our community members can thrive. Violence, intimidation, discrimination, bullying, and any behaviors that prevent teaching, learning, or research are antithetical 
 to our values and our mission.
 To create an environment driven by our values and principles, leadership 
-must *engage across our community*, listening to and learning from 
+must engage across our community, listening to and learning from 
 students, faculty, staff, alumni, and neighbors. This work will take the 
 form of regular communications; meetings with faculty, students, staff, 
 and alumni; alongside public events, including town halls and panel 
@@ -1721,27 +1422,21 @@
 participate in a discussion. I know that the deans and administrative 
 leadership teams join me in this commitment.
 Our university has extraordinary faculty whose scholarship, research and 
-academic excellence provide a critical resource for *advancing knowledge 
-and understanding* at this pivotal time. I am eager to work with our 
+academic excellence provide a critical resource for advancing knowledge 
+and understanding at this pivotal time. I am eager to work with our 
 faculty to leverage our greatest strengths today towards the educational 
 mission. Many thanks to several of the deans who are working together 
 with our faculty to propose innovative approaches in this area. At the 
-same time, we will expand the Campus Climate Working Group, initiated by 
-our Provost, Angela Olinto, that brings together voices from across our 
+same time, we will expand the Campus Climate Working Group, initiated by our Provost, Angela Olinto, that brings together voices from across our 
 more than two dozen schools and units. This group focuses on ways to 
 advance our shared understanding through academic programming, 
 workshops, training, community-building and skills-based programming. I 
 am confident that bringing together experience, resources, and expertise 
 across Columbia will make our efforts more impactful.
-There is no doubt that redoubling our commitment to *addressing 
-discrimination and harassment* and the toll they take will be essential 
+There is no doubt that redoubling our commitment to addressing 
+discrimination and harassment and the toll they take will be essential 
 going forward. Under the leadership of Provost Olinto, we are bringing 
-several functions together in a new Office of Institutional Equity 
-&lt;http://institutionalequity.columbia.edu/&gt; led by Vice Provost Laura 
-Kirschstein. The Office will serve as a centralized resource for 
-addressing all reports of discrimination and discriminatory harassment, 
-including reports that involve alleged violations of Title VI and Title 
-VII, reports that involve alleged violations of Title IX and the 
+several functions together in a new Office of Institutional Equity led by Vice Provost Laura Kirschstein. The Office will serve as a centralized resource for addressing all reports of discrimination and discriminatory harassment, including reports that involve alleged violations of Title VI and Title VII, reports that involve alleged violations of Title IX and the 
 University's Gender Based Misconduct Policy, as well as reports that 
 relate to violations of the Protection of Minors Policy. It will serve 
 as a streamlined center with the express goal of ensuring that reports 
@@ -1749,7 +1444,7 @@
 personally committed to making this process more effective for every 
 member of our community who reports such discrimination. Our Provost 
 will be providing further details on this important development.
-Effectively *managing protests and demonstrations* allows us to advance 
+Effectively managing protests and demonstrations allows us to advance 
 our educational and research missions while enabling free speech and 
 debate. My discussions have made it clear that effective management 
 requires a commitment to a fair application of the rules and thoughtful 
@@ -1761,9 +1456,7 @@
 function effectively, efficiently, and equitably to ensure that we are 
 able to achieve our mission and uphold our values and principles. At the 
 same time, I am grateful that the Inclusive Public Safety Advisory 
-Committee &lt;https://universitylife.columbia.edu/inclusive-public-safety&gt; 
-will be reenergized to fulfill its charge of providing guidance on how 
-Public Safety practices and policies can best support a safe and an 
+Committee will be reenergized to fulfill its charge of providing guidance on how Public Safety practices and policies can best support a safe and an 
 inclusive campus. As an immediate step, I have asked the Committee to 
 conduct listening sessions with our community. Please stay tuned for 
 more on how to participate in those sessions and for more information on 
@@ -1778,193 +1471,7 @@
 hard—work, and it requires each of us to do our part. I am confident we 
 can do what is needed.
 I am eager to welcome our new students and to greet all of you returning 
-to campus as we begin the new semester.
-All my best,
-Katrina A. Armstrong
-Interim President
-Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear members of the Columbia community,
-I am deeply honored to be called to serve as Interim President of our
-beloved institution. This role comes at a pivotal moment for Columbia, and
-I am excited and humbled by the opportunity to contribute to our collective
-journey. With profound respect for Columbia's storied history and an
-unwavering commitment to its future, I look forward to working with you to
-achieve our shared goals.
-Challenging times present both the opportunity and the responsibility for
-serious leadership to emerge from every group and individual within a
-community. This is such a time at Columbia. As I step into this role, I am
-acutely aware of the trials the University has faced over the past year. We
-should neither understate their significance, nor allow them to define who
-we are and what we will become. The familiar excitement and promise of a
-new academic year are informed this year by the presence of change and
-continuing concerns, but also by the immense opportunity to look forward,
-to join together for the laudable mission we are here to serve, and to
-become our best selves individually and institutionally. Never has it been
-more important to train leaders capable of elevating society and addressing
-the complexity of modern life. Columbia University has a long history of
-meeting the moment, and I have faith that we will do so once again. I ask
-each of you to join me in this critically important work fueled by the
-enthusiasm for what we can accomplish together. Through our collective
-effort, I am confident we will succeed.
-Much of this work will fall to the Columbia faculty. You are the ultimate
-keepers of the institution's values and the stewards of its long and proud
-history. The habit of critical thinking and humility that gives birth to
-tolerance of contrary points of view is the most essential lesson taught in
-Columbia's classrooms and the intellectual common ground that unifies the
-many scholarly pursuits found across our campuses. Physicians learn this
-philosophical approach quickly as it can often be the difference between
-life and death. My leadership of Columbia University Irving Medical Center
-(CUIMC) has been grounded in consistent engagement with the entire faculty
-across all four schools, and that will again be the case during my time as
-your Interim University President.
-I assume this role able to stand on the shoulders of our two most recent
-presidents, Minouche Shafik and Lee C. Bollinger, whose dedication to
-Columbia is boundless, and I take comfort in knowing they will be available
-to me and to Columbia going forward. The University exists because of the
-love for the institution expressed and the contributions made by countless
-talented individuals over many decades, particularly our faithful alumni.
-First among these, in my experience, is P. Roy Vagelos, a visionary leader
-and supremely generous benefactor, whose friendship I have relied on
-throughout my time at Columbia and whom I must recognize and thank here.
-I have been privileged to spend my professional life at the greatest
-research universities in the United States, serving as a teacher,
-researcher, attending physician, department chair, administrative leader,
-dean, and, most recently, head of CUIMC, one of the nation's greatest
-academic medical centers. I fully appreciate the profound responsibility of
-meeting the needs of the many constituencies that make Columbia University
-the renowned leader in higher education that it is. With optimism and
-resolve, let us move forward together, embracing the opportunity to renew
-our vision and strengthen our community.
-All my best,
-Katrina A. Armstrong
-Interim President
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear fellow members of the Columbia community:
-I am writing heartbroken to inform you that we had federal agents from the
-Department of Homeland Security (DHS) in two University residences tonight.
-No one was arrested or detained. No items were removed, and no further
-action was taken.
-Federal agents from the DHS served Columbia University with two judicial
-search warrants signed by a federal magistrate judge authorizing DHS to
-enter non-public areas of the University and conduct searches of two
-student rooms.
-The University has a clear protocol
-&lt;https://publicsafety.columbia.edu/content/protocol-potential-visits-campus-us-immigration-and-customs-enforcement-ice-agents&gt;
-in place. Consistent with this protocol, our longstanding practice, and the
-practices of cities and institutions throughout the country, the University
-requires that law enforcement have a judicial warrant to enter non-public
-University areas, including residential University buildings. Tonight, that
-threshold was met, and the University is obligated to comply with the law.
-Our University Public Safety was present at all times.
-Columbia continues to make every effort to ensure that our campus,
-students, faculty, and staff are safe. Columbia is committed to upholding
-the law, and we expect city, state, and federal agencies to do the same.
-I understand the immense stress our community is under. Despite the
-unprecedented challenges, Columbia University will remain a place where the
-pursuit of knowledge is cherished and fiercely protected, where the rule of
-law and due process is respected and never taken for granted, and where all
-members of our community are valued and able to thrive. These are the
-principles we uphold and that guide us every day.
-For students in need of support, I've included a list of University
-resources below.
-Standing together for Columbia,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear Columbia Community,
-I write to you at a challenging moment for our community. Columbia 
-University exists to serve the United States and the world, by teaching, 
-creating, and advancing knowledge. We pursue that mission through 
-freedom of expression, open inquiry, a wide range of perspectives, and 
-respectful debate. These are Columbia's values, they are America's 
-values, they are essential to a functioning democracy, and we will fight 
-for them. We do this for our students and for our future.
-Here is what that means in this particular moment:
-  * *We will work tirelessly to fulfill our mission*. We are taking a
-    methodical and thoughtful approach to addressing the multitude of
-    challenges ahead of us. We are engaged with several federal agencies
-    and are doing all we can to be responsive to their legitimate
-    concerns and to take corrective action, under the law, to restore
-    funding.
-  * *We will support our community*. I understand the distress that many
-    of you are feeling about the presence of U.S. Immigration and
-    Customs Enforcement (ICE) agents in the streets around campus. I
-    feel it too and am working with our team to manage the response.
-    Resources for students are listed below.
-  * *We will follow the law*, as has always been the case, and rumors
-    suggesting that any member of Columbia leadership requested the
-    presence of U.S. Immigration and Customs Enforcement (ICE) agents on
-    or near campus are false. It remains the long-standing practice of
-    the University, and the practice of cities and institutions
-    throughout the country, that law enforcement must have a judicial
-    warrant to enter non-public University areas, including residential
-    University buildings.
-  * *We are deeply committed to freedom of speech* as a fundamental
-    value that we must uphold as a community—citizens and non-citizens
-    alike. Vigorous and open debate, consistent with our rules, is
-    central to achieving our academic mission. We must welcome the
-    widest possible range of ideas, perspectives, and life experiences
-    from all members of our community whether American or International.
-    Our mission at Columbia also requires that we treat one another with
-    respect, which enables us to disagree without being disagreeable. We
-    need to do so in an environment free from discrimination.
-I am proud of Columbia's unwavering commitment to excellence, and our 
-historic and ongoing contributions to the United States and the world, 
-from technology, to medicine, to the humanities, to the laws 
-underpinning our democracy itself. I ask for your continued support and 
-patience. The only way to navigate this moment is together, as a united 
-community.
-All eyes are on Columbia at present. It falls to us to ensure our 
-University, and indeed the values of higher education more broadly, 
-survive and thrive.
-Sincerely,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York
-</t>
-  </si>
-  <si>
-    <t>Dear Members of the Columbia community:
-In September, I announced the creation of a President's Advisory 
-Committee on Institutional Voice 
-&lt;https://president.columbia.edu/news/appointment-co-chairs-presidents-advisory-committee-institutional-voice&gt; 
-to provide me with a set of recommendations on the proper role of 
-institutional voice in advancing Columbia's academic mission and its 
-commitment to open inquiry and free expression. I am writing now with an 
-update on this critical work.
-I am pleased to share that the Committee has begun its work, including 
-developing an engagement strategy and holding meetings with faculty, 
-students, administrators, and staff from across the University. The 
-Committee anticipates completing its work and providing a report to me 
-by the end of the current academic year. The full roster of Committee 
-members is listed below. They include thoughtful and experienced faculty 
-from departments and schools across our campuses, and I am very grateful 
-to them for agreeing to do this challenging and urgently needed work.
-The Committee has also established a website 
-&lt;https://www.columbia.edu/content/members-committee-institutional-voice&gt;, 
-which will be a resource for further information and updates. It will 
-welcome input and feedback from members of the Columbia community, so 
-please get in touch with them at institutionalvoice@columbia.edu if you 
-would like to share your thoughts and insights.
-I offer my deepest thanks to the two distinguished Co-Chairs, Daniel 
-Abebe, Dean of Columbia Law School and Lucy G. Moses Professor of Law, 
-and Mark Mazower, Ira D. Wallach Professor of World Order Studies, and 
-to all the members of the Committee. We are very fortunate to have their 
-deliberations guide us in this important project.
-All my best,
-Katrina Armstrong
-Interim President, Columbia University in the City of New York</t>
-  </si>
-  <si>
-    <t>A Message from Katrina Armstrong</t>
-  </si>
-  <si>
-    <t>Content</t>
+to campus as we begin the new semester.</t>
   </si>
 </sst>
 </file>
@@ -2023,12 +1530,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2335,10 +1845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2354,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2362,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>58</v>
@@ -2373,7 +1883,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>59</v>
@@ -2384,7 +1894,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>60</v>
@@ -2395,10 +1905,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2406,10 +1916,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2417,10 +1927,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2428,10 +1938,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2439,10 +1949,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2450,10 +1960,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2461,10 +1971,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2472,10 +1982,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2483,10 +1993,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2494,10 +2004,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2505,10 +2015,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2516,10 +2026,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2527,10 +2037,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2538,10 +2048,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2549,10 +2059,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2560,32 +2070,32 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2593,10 +2103,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2604,10 +2114,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2615,10 +2125,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2626,10 +2136,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2637,10 +2147,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
@@ -2648,32 +2158,21 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>